<commit_message>
Fix format and examples.
</commit_message>
<xml_diff>
--- a/doc/databasesamples.xlsx
+++ b/doc/databasesamples.xlsx
@@ -181,13 +181,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.94"/>
   </cols>

</xml_diff>